<commit_message>
Removendo falhas da deteccao de colisao
</commit_message>
<xml_diff>
--- a/Ex11_Colisão/ver/PontosColisão.xlsx
+++ b/Ex11_Colisão/ver/PontosColisão.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="15315" windowHeight="5700"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="15315" windowHeight="5700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="24">
   <si>
     <t>p1</t>
   </si>
@@ -92,7 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +117,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="35"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="35"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +163,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -237,11 +258,161 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -261,7 +432,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -305,6 +475,92 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,412 +863,815 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E4:U27"/>
+  <dimension ref="C2:AA31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="10" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="25" width="4.42578125" customWidth="1"/>
+    <col min="26" max="27" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="3:27" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="L3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="L4" s="6"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="31"/>
+      <c r="T4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="T4" s="7" t="s">
+      <c r="X4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="5:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="1"/>
+      <c r="J5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="L5" s="6"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="31"/>
+      <c r="S5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="T5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="13" t="s">
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="U5" s="10" t="s">
+      <c r="Y5" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E6" s="6"/>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="4"/>
-      <c r="M6" s="11"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
-      <c r="T6" s="4"/>
-    </row>
-    <row r="7" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="I6" s="3"/>
+      <c r="J6" s="4"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="31"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="4"/>
+    </row>
+    <row r="7" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E7" s="6"/>
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="4"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="4"/>
-    </row>
-    <row r="8" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="I7" s="3"/>
+      <c r="J7" s="4"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="50"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="39"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="4"/>
+    </row>
+    <row r="8" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="6"/>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="4"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="4"/>
-    </row>
-    <row r="9" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
+      <c r="L8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="52"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="S8" s="6"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="4"/>
+    </row>
+    <row r="9" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E9" s="6"/>
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="3"/>
+      <c r="I9" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="I9" s="22"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="25" t="s">
+      <c r="J9" s="21"/>
+      <c r="M9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="S9" s="6"/>
+      <c r="T9" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="R9" s="22"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="4"/>
-    </row>
-    <row r="10" spans="5:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U9" s="21"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="4"/>
+    </row>
+    <row r="10" spans="3:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>3</v>
       </c>
       <c r="G10" s="5"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="10" t="s">
+      <c r="H10" s="5"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="S10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="26" t="s">
+      <c r="T10" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="R10" s="24"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="15" t="s">
+      <c r="U10" s="23"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="U10" s="10" t="s">
+      <c r="Y10" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="5:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="L11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-      <c r="O11" s="7" t="s">
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="Q11" s="8" t="s">
+      <c r="T11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="T11" s="7" t="s">
+      <c r="X11" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="5:21" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="J12" s="9" t="s">
+    <row r="12" spans="3:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="L12" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="13" t="s">
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="S12" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="J13" s="9"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="19"/>
-      <c r="P13" s="10"/>
-    </row>
-    <row r="14" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="J14" s="9"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="10"/>
-    </row>
-    <row r="15" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="J15" s="9"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="10"/>
-    </row>
-    <row r="16" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="J16" s="9"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="10"/>
-    </row>
-    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="J17" s="9"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="10"/>
-    </row>
-    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="J18" s="9"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="10"/>
-    </row>
-    <row r="19" spans="5:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J19" s="9" t="s">
+      <c r="V12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z12" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="3:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="10"/>
+      <c r="U13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="V13" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13" s="44"/>
+      <c r="X13" s="29"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="3:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="6"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="37"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="10"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="46"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="31"/>
+    </row>
+    <row r="15" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C15" s="6"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="31"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="10"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="30"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="31"/>
+    </row>
+    <row r="16" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="C16" s="6"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="31"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="18"/>
+      <c r="S16" s="10"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="30"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="31"/>
+    </row>
+    <row r="17" spans="3:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="6"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="39"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="10"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="W17" s="50"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="31"/>
+    </row>
+    <row r="18" spans="3:27" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="9"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="10"/>
+      <c r="U18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="V18" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="W18" s="52"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="32"/>
+      <c r="Z18" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA18" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="3:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="L19" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="15" t="s">
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="P19" s="10" t="s">
+      <c r="S19" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="5:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z19" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="J20" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="L20" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="8"/>
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
-      <c r="O20" s="7" t="s">
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="Q20" s="8" t="s">
+      <c r="T20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="T20" s="7" t="s">
+      <c r="X20" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="5:21" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:27" ht="18.75" x14ac:dyDescent="0.25">
       <c r="E21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="11" t="s">
         <v>0</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="29" t="s">
-        <v>1</v>
-      </c>
+      <c r="H21" s="1"/>
       <c r="I21" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="P21" s="9" t="s">
+      <c r="S21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="27" t="s">
+      <c r="T21" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="R21" s="28"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="13" t="s">
+      <c r="U21" s="27"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="U21" s="10" t="s">
+      <c r="Y21" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="5:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E22" s="6"/>
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="24"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="3"/>
-      <c r="T22" s="4"/>
-    </row>
-    <row r="23" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="H22" s="3"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="23"/>
+      <c r="M22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S22" s="6"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="4"/>
+    </row>
+    <row r="23" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E23" s="6"/>
       <c r="F23" s="2"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="4"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="4"/>
-    </row>
-    <row r="24" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="I23" s="3"/>
+      <c r="J23" s="4"/>
+      <c r="L23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" s="44"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="53" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S23" s="6"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="4"/>
+    </row>
+    <row r="24" spans="3:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E24" s="6"/>
       <c r="F24" s="2"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="4"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="2"/>
-      <c r="R24" s="3"/>
-      <c r="S24" s="3"/>
-      <c r="T24" s="4"/>
-    </row>
-    <row r="25" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="I24" s="3"/>
+      <c r="J24" s="4"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="37"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="4"/>
+    </row>
+    <row r="25" spans="3:27" x14ac:dyDescent="0.25">
       <c r="E25" s="6"/>
       <c r="F25" s="2"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="4"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="3"/>
-      <c r="S25" s="3"/>
-      <c r="T25" s="4"/>
-    </row>
-    <row r="26" spans="5:21" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="3"/>
+      <c r="J25" s="4"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="31"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="4"/>
+    </row>
+    <row r="26" spans="3:27" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E26" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="13" t="s">
         <v>3</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="15" t="s">
+      <c r="I26" s="5"/>
+      <c r="J26" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="K26" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="P26" s="9" t="s">
+      <c r="L26" s="6"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="31"/>
+      <c r="S26" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="14" t="s">
+      <c r="T26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="15" t="s">
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="U26" s="10" t="s">
+      <c r="Y26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:27" x14ac:dyDescent="0.25">
       <c r="F27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I27" s="7" t="s">
+      <c r="J27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Q27" s="8" t="s">
+      <c r="L27" s="6"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="31"/>
+      <c r="T27" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="T27" s="7" t="s">
+      <c r="X27" s="7" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="28" spans="3:27" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M28" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="R28" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="3:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="3:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="3:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="H9:I10"/>
-    <mergeCell ref="Q9:R10"/>
-    <mergeCell ref="Q21:R22"/>
-    <mergeCell ref="H21:I22"/>
+  <mergeCells count="12">
+    <mergeCell ref="V17:W18"/>
+    <mergeCell ref="V13:W14"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="P23:Q24"/>
+    <mergeCell ref="M23:N24"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="T9:U10"/>
+    <mergeCell ref="T21:U22"/>
+    <mergeCell ref="I21:J22"/>
+    <mergeCell ref="G17:H18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.140625" style="55" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="55" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B4" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B5" s="60"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="58"/>
+    </row>
+    <row r="6" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B6" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="56"/>
+      <c r="D6" s="57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B7" s="60"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="58"/>
+    </row>
+    <row r="8" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B8" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="56"/>
+      <c r="D8" s="57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B9" s="60"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="58"/>
+    </row>
+    <row r="10" spans="2:4" ht="46.5" thickBot="1" x14ac:dyDescent="0.75">
+      <c r="B10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>